<commit_message>
Initial commit in development
</commit_message>
<xml_diff>
--- a/config/config-sra-test.xlsx
+++ b/config/config-sra-test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih-my.sharepoint.com/personal/cherikhsr_nih_gov/Documents/cidc/pycharm-workspace/cidc_atac/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherikhsr/Documents/GitHub/cidc_atac/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{1B1FD6D5-973C-3E41-809E-7332B58C6084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DAAE3EE-9F61-5B4F-A58E-0964AD57F8A5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43A89C7-01B8-454A-A47E-52F3212D4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="30900" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1862,10 +1862,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2737,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2798,7 +2794,7 @@
         <v>109</v>
       </c>
       <c r="C5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updates some output paths in test config
</commit_message>
<xml_diff>
--- a/config/config-sra-test.xlsx
+++ b/config/config-sra-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherikhsr/Documents/GitHub/cidc_atac/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43A89C7-01B8-454A-A47E-52F3212D4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1D2366-DDDB-8F40-88CE-1131E549999D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="30900" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="30180" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -1441,15 +1441,6 @@
     </r>
   </si>
   <si>
-    <t>/home/cherikhsr/atac_test_output</t>
-  </si>
-  <si>
-    <t>/home/cherikhsr/atac_test_output/analysis</t>
-  </si>
-  <si>
-    <t>annot genome input bam rseqc fastqc tmp cutadapt rqual_filter progress benchmark log info cnv peak chipqc</t>
-  </si>
-  <si>
     <t>peak_mode</t>
   </si>
   <si>
@@ -1645,6 +1636,15 @@
   </si>
   <si>
     <t>Fastq File name (uncompressed or gzip compressed); For local files use path from root; for Amazon S3 files, use s3://&lt;bucket&gt;/&lt;key&gt;; for SRA runs, use the accession number (i.e. SRR2057712). Files separated by semi-colons will be merged before processing. If using SRR that are paired end copy the same accession into the fastq_file_2 column as well</t>
+  </si>
+  <si>
+    <t>/home/cherikhsr_nih_gov/atac_test_output</t>
+  </si>
+  <si>
+    <t>/home/cherikhsr_nih_gov/atac_test_output/analysis</t>
+  </si>
+  <si>
+    <t>benchmark log info progress genome annot input cutadapt rqual_filter bam rseqc fastqc cnv peak chipqc</t>
   </si>
 </sst>
 </file>
@@ -2206,10 +2206,10 @@
         <v>60</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>61</v>
@@ -2263,10 +2263,10 @@
         <v>37</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>39</v>
@@ -2278,7 +2278,7 @@
         <v>41</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>20</v>
@@ -2355,7 +2355,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2363,27 +2363,27 @@
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="P4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="Q4" s="26"/>
     </row>
     <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2391,27 +2391,27 @@
         <v>2</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="Q5" s="26"/>
     </row>
     <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2419,26 +2419,26 @@
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2446,26 +2446,26 @@
         <v>2</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2473,26 +2473,26 @@
         <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="O8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="P8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2500,16 +2500,16 @@
         <v>2</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="O9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2763,7 +2763,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -2774,7 +2774,7 @@
         <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2821,21 +2821,21 @@
     </row>
     <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C9" s="6">
         <v>73</v>
@@ -2843,10 +2843,10 @@
     </row>
     <row r="10" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C10" s="6">
         <v>37</v>
@@ -2854,10 +2854,10 @@
     </row>
     <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C11" s="6">
         <v>0.05</v>
@@ -2893,7 +2893,7 @@
         <v>139</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2975,13 +2975,13 @@
     </row>
     <row r="22" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3030,7 +3030,7 @@
         <v>124</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -3054,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3084,7 +3084,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">

</xml_diff>